<commit_message>
tooltip and text changes
</commit_message>
<xml_diff>
--- a/docss/trend/cyprus/E_huntington.xlsx
+++ b/docss/trend/cyprus/E_huntington.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELENA\Documents\IC3\ic3desarrollo\docss\trend\cyprus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos de Elena\Documents\GitHub\ic3desarrollo\docss\trend\cyprus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -187,6 +187,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -239,6 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1558,7 +1562,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,13 +1585,13 @@
       <c r="A2">
         <v>2004</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="7">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1601,7 +1605,7 @@
       <c r="C3">
         <v>0.28100000000000003</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1612,7 +1616,7 @@
       <c r="B4">
         <v>0.14899999999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>0</v>
       </c>
       <c r="D4">
@@ -1623,13 +1627,13 @@
       <c r="A5">
         <v>2007</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1640,7 +1644,7 @@
       <c r="B6">
         <v>0.25</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6">
@@ -1651,13 +1655,13 @@
       <c r="A7">
         <v>2009</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1668,7 +1672,7 @@
       <c r="B8">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <v>0</v>
       </c>
       <c r="D8">
@@ -1679,13 +1683,13 @@
       <c r="A9">
         <v>2011</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1696,7 +1700,7 @@
       <c r="B10">
         <v>0.1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10">
@@ -1713,7 +1717,7 @@
       <c r="C11">
         <v>0.191</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>0</v>
       </c>
     </row>

</xml_diff>